<commit_message>
changed list of files order and test
</commit_message>
<xml_diff>
--- a/input_data/TableForReferenceScData_11072023.xlsx
+++ b/input_data/TableForReferenceScData_11072023.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://virginiatech-my.sharepoint.com/personal/songli_vt_edu/Documents/A_NinaProjects_2022/SingleCellCrossSpecies_2022/NaturePlantLetter_FinalVerion_ByNov302023/OMGBrowser_Test_11072023/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://virginiatech-my.sharepoint.com/personal/songli_vt_edu/Documents/A_NinaProjects_2022/SingleCellCrossSpecies_2022/OMGbrowser_Final_11132023/OMGBrowser/input_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="100" documentId="8_{2F6F3F6C-A327-E44C-B537-9585B5992508}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2B773D4E-B265-8140-B131-30FCC04A1747}"/>
+  <xr:revisionPtr revIDLastSave="102" documentId="8_{2F6F3F6C-A327-E44C-B537-9585B5992508}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{118C7A36-4316-CC4C-B25C-F549A752CD78}"/>
   <bookViews>
-    <workbookView xWindow="2680" yWindow="1380" windowWidth="28040" windowHeight="17440" xr2:uid="{C17EE9DD-9FFE-464F-B37F-5C4FA6E87D5B}"/>
+    <workbookView xWindow="10880" yWindow="2820" windowWidth="31920" windowHeight="17440" xr2:uid="{C17EE9DD-9FFE-464F-B37F-5C4FA6E87D5B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -557,8 +557,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88ABD0FC-1E3D-C049-90D3-7F47A0518D42}">
   <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="223" zoomScaleNormal="223" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="223" zoomScaleNormal="223" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19:XFD19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -589,67 +589,61 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" t="s">
-        <v>6</v>
+        <v>33</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" t="s">
-        <v>9</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D3" t="s">
         <v>8</v>
       </c>
       <c r="E3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D4" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="E4" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="B5" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C5" t="s">
-        <v>52</v>
+        <v>15</v>
       </c>
       <c r="D5" t="s">
-        <v>8</v>
+        <v>16</v>
+      </c>
+      <c r="E5" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -657,7 +651,7 @@
         <v>19</v>
       </c>
       <c r="B6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C6" t="s">
         <v>52</v>
@@ -671,7 +665,7 @@
         <v>19</v>
       </c>
       <c r="B7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C7" t="s">
         <v>52</v>
@@ -685,7 +679,7 @@
         <v>19</v>
       </c>
       <c r="B8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C8" t="s">
         <v>52</v>
@@ -699,7 +693,7 @@
         <v>19</v>
       </c>
       <c r="B9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C9" t="s">
         <v>52</v>
@@ -713,7 +707,7 @@
         <v>19</v>
       </c>
       <c r="B10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C10" t="s">
         <v>52</v>
@@ -724,87 +718,84 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B11" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="C11" t="s">
-        <v>36</v>
+        <v>52</v>
       </c>
       <c r="D11" t="s">
         <v>8</v>
-      </c>
-      <c r="E11" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B12" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="C12" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D12" t="s">
         <v>8</v>
       </c>
       <c r="E12" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B13" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C13" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D13" t="s">
         <v>8</v>
       </c>
       <c r="E13" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B14" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="C14" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="D14" t="s">
         <v>8</v>
       </c>
       <c r="E14" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B15" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="C15" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="D15" t="s">
         <v>8</v>
       </c>
       <c r="E15" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
@@ -812,41 +803,50 @@
         <v>30</v>
       </c>
       <c r="B16" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C16" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D16" t="s">
         <v>8</v>
       </c>
       <c r="E16" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B17" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="C17" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="D17" t="s">
         <v>8</v>
       </c>
       <c r="E17" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>33</v>
+        <v>32</v>
+      </c>
+      <c r="B18" t="s">
+        <v>55</v>
       </c>
       <c r="C18" t="s">
-        <v>52</v>
+        <v>53</v>
+      </c>
+      <c r="D18" t="s">
+        <v>8</v>
+      </c>
+      <c r="E18" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">

</xml_diff>